<commit_message>
feat: it6801 fit 1920x1280@30, debayer error
</commit_message>
<xml_diff>
--- a/sch/pin.xlsx
+++ b/sch/pin.xlsx
@@ -1491,11 +1491,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1505,15 +1505,81 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1521,7 +1587,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1544,37 +1633,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1589,37 +1648,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1633,23 +1662,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1676,42 +1690,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1724,7 +1702,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,13 +1750,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1760,73 +1858,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1838,25 +1870,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2089,16 +2103,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2163,6 +2177,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2171,172 +2200,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2370,6 +2384,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2412,13 +2435,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2876,8 +2899,8 @@
   <sheetPr/>
   <dimension ref="A2:AA74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2910,17 +2933,17 @@
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" ht="13.5" spans="2:27">
       <c r="B4" s="4" t="s">
@@ -2932,43 +2955,43 @@
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="34" t="s">
+      <c r="I4" s="33"/>
+      <c r="J4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="36" t="s">
+      <c r="L4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="46" t="s">
+      <c r="Q4" s="48"/>
+      <c r="R4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="47" t="s">
+      <c r="S4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="31" t="s">
+      <c r="U4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="31" t="s">
+      <c r="V4" s="55"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="53"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="56"/>
     </row>
     <row r="5" ht="13.5" spans="2:27">
       <c r="B5" s="7"/>
@@ -2978,39 +3001,39 @@
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
-      <c r="Q5" s="37" t="s">
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
+      <c r="Q5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="48" t="s">
+      <c r="R5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="49" t="s">
+      <c r="S5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="34" t="s">
+      <c r="U5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="V5" s="55" t="s">
+      <c r="V5" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="W5" s="56" t="s">
+      <c r="W5" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="34" t="s">
+      <c r="X5" s="57"/>
+      <c r="Y5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="Z5" s="55" t="s">
+      <c r="Z5" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AA5" s="56" t="s">
+      <c r="AA5" s="59" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3025,46 +3048,46 @@
       <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="40" t="s">
+      <c r="I6" s="33"/>
+      <c r="J6" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="50" t="s">
+      <c r="Q6" s="43"/>
+      <c r="R6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="51" t="s">
+      <c r="S6" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="U6" s="57" t="s">
+      <c r="U6" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="48" t="s">
+      <c r="V6" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="49" t="s">
+      <c r="W6" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="57" t="s">
+      <c r="X6" s="57"/>
+      <c r="Y6" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="48" t="s">
+      <c r="Z6" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AA6" s="49" t="s">
+      <c r="AA6" s="52" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3075,46 +3098,46 @@
       <c r="F7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="40" t="s">
+      <c r="I7" s="33"/>
+      <c r="J7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="50" t="s">
+      <c r="Q7" s="43"/>
+      <c r="R7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="S7" s="51" t="s">
+      <c r="S7" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="U7" s="40" t="s">
+      <c r="U7" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="V7" s="50" t="s">
+      <c r="V7" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="W7" s="51" t="s">
+      <c r="W7" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="40" t="s">
+      <c r="X7" s="57"/>
+      <c r="Y7" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="Z7" s="50" t="s">
+      <c r="Z7" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="AA7" s="51" t="s">
+      <c r="AA7" s="54" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3131,42 +3154,42 @@
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="40" t="s">
+      <c r="I8" s="33"/>
+      <c r="J8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="51"/>
-      <c r="U8" s="58" t="s">
+      <c r="Q8" s="43"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="54"/>
+      <c r="U8" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="V8" s="50" t="s">
+      <c r="V8" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="W8" s="51" t="s">
+      <c r="W8" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="58" t="s">
+      <c r="X8" s="57"/>
+      <c r="Y8" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="Z8" s="50" t="s">
+      <c r="Z8" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="AA8" s="51" t="s">
+      <c r="AA8" s="54" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3181,48 +3204,48 @@
       <c r="F9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="40" t="s">
+      <c r="I9" s="33"/>
+      <c r="J9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="Q9" s="40" t="s">
+      <c r="Q9" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="R9" s="50" t="s">
+      <c r="R9" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="51" t="s">
+      <c r="S9" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="U9" s="40" t="s">
+      <c r="U9" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="V9" s="50" t="s">
+      <c r="V9" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="W9" s="51" t="s">
+      <c r="W9" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="40" t="s">
+      <c r="X9" s="57"/>
+      <c r="Y9" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="Z9" s="50" t="s">
+      <c r="Z9" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="AA9" s="51" t="s">
+      <c r="AA9" s="54" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3237,46 +3260,46 @@
       <c r="F10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="40" t="s">
+      <c r="I10" s="33"/>
+      <c r="J10" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="50" t="s">
+      <c r="Q10" s="43"/>
+      <c r="R10" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="S10" s="51" t="s">
+      <c r="S10" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="U10" s="58" t="s">
+      <c r="U10" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="V10" s="50" t="s">
+      <c r="V10" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="W10" s="51" t="s">
+      <c r="W10" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="X10" s="54"/>
-      <c r="Y10" s="58" t="s">
+      <c r="X10" s="57"/>
+      <c r="Y10" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="Z10" s="50" t="s">
+      <c r="Z10" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="AA10" s="51" t="s">
+      <c r="AA10" s="54" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3291,46 +3314,46 @@
       <c r="F11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="40" t="s">
+      <c r="I11" s="33"/>
+      <c r="J11" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="50" t="s">
+      <c r="Q11" s="43"/>
+      <c r="R11" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="S11" s="51" t="s">
+      <c r="S11" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="U11" s="40" t="s">
+      <c r="U11" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="50" t="s">
+      <c r="V11" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="51" t="s">
+      <c r="W11" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="X11" s="54"/>
-      <c r="Y11" s="40" t="s">
+      <c r="X11" s="57"/>
+      <c r="Y11" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="Z11" s="50" t="s">
+      <c r="Z11" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="AA11" s="51" t="s">
+      <c r="AA11" s="54" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3345,46 +3368,46 @@
       <c r="F12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="40" t="s">
+      <c r="I12" s="33"/>
+      <c r="J12" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="41" t="s">
+      <c r="K12" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="50" t="s">
+      <c r="Q12" s="43"/>
+      <c r="R12" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="S12" s="51" t="s">
+      <c r="S12" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="U12" s="58" t="s">
+      <c r="U12" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="V12" s="50" t="s">
+      <c r="V12" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="W12" s="51" t="s">
+      <c r="W12" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="X12" s="54"/>
-      <c r="Y12" s="58" t="s">
+      <c r="X12" s="57"/>
+      <c r="Y12" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="Z12" s="50" t="s">
+      <c r="Z12" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="AA12" s="51" t="s">
+      <c r="AA12" s="54" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3399,46 +3422,46 @@
       <c r="F13" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="40" t="s">
+      <c r="I13" s="33"/>
+      <c r="J13" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="50" t="s">
+      <c r="Q13" s="43"/>
+      <c r="R13" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="S13" s="51" t="s">
+      <c r="S13" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="U13" s="40" t="s">
+      <c r="U13" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="V13" s="50" t="s">
+      <c r="V13" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="W13" s="51" t="s">
+      <c r="W13" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="X13" s="54"/>
-      <c r="Y13" s="40" t="s">
+      <c r="X13" s="57"/>
+      <c r="Y13" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="Z13" s="50" t="s">
+      <c r="Z13" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="AA13" s="51" t="s">
+      <c r="AA13" s="54" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3453,46 +3476,46 @@
       <c r="F14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="40" t="s">
+      <c r="I14" s="33"/>
+      <c r="J14" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="50" t="s">
+      <c r="Q14" s="43"/>
+      <c r="R14" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="S14" s="51" t="s">
+      <c r="S14" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="U14" s="58" t="s">
+      <c r="U14" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="V14" s="50" t="s">
+      <c r="V14" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="W14" s="51" t="s">
+      <c r="W14" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="58" t="s">
+      <c r="X14" s="57"/>
+      <c r="Y14" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="Z14" s="50" t="s">
+      <c r="Z14" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="AA14" s="51" t="s">
+      <c r="AA14" s="54" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3503,46 +3526,46 @@
       <c r="F15" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="40" t="s">
+      <c r="I15" s="33"/>
+      <c r="J15" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="50" t="s">
+      <c r="Q15" s="43"/>
+      <c r="R15" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="S15" s="51" t="s">
+      <c r="S15" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="U15" s="40" t="s">
+      <c r="U15" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="V15" s="50" t="s">
+      <c r="V15" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="W15" s="51" t="s">
+      <c r="W15" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="X15" s="54"/>
-      <c r="Y15" s="40" t="s">
+      <c r="X15" s="57"/>
+      <c r="Y15" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="Z15" s="50" t="s">
+      <c r="Z15" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="AA15" s="51" t="s">
+      <c r="AA15" s="54" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3557,26 +3580,26 @@
         <v>127</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="28"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="50" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="31"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="S16" s="51" t="s">
+      <c r="S16" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="U16" s="40"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="54"/>
-      <c r="Y16" s="40"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="51"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="53"/>
+      <c r="AA16" s="54"/>
     </row>
     <row r="17" spans="2:27">
       <c r="B17" s="7"/>
@@ -3589,46 +3612,46 @@
       <c r="F17" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="40" t="s">
+      <c r="I17" s="33"/>
+      <c r="J17" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="L17" s="28" t="s">
+      <c r="L17" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="50" t="s">
+      <c r="Q17" s="43"/>
+      <c r="R17" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="S17" s="51" t="s">
+      <c r="S17" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="U17" s="40" t="s">
+      <c r="U17" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="V17" s="50" t="s">
+      <c r="V17" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="W17" s="51" t="s">
+      <c r="W17" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="40" t="s">
+      <c r="X17" s="57"/>
+      <c r="Y17" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="Z17" s="50" t="s">
+      <c r="Z17" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="AA17" s="51" t="s">
+      <c r="AA17" s="54" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3643,46 +3666,46 @@
       <c r="F18" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="40" t="s">
+      <c r="I18" s="33"/>
+      <c r="J18" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="K18" s="41" t="s">
+      <c r="K18" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="L18" s="28" t="s">
+      <c r="L18" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="50" t="s">
+      <c r="Q18" s="43"/>
+      <c r="R18" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="S18" s="51" t="s">
+      <c r="S18" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="U18" s="40" t="s">
+      <c r="U18" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="V18" s="50" t="s">
+      <c r="V18" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="W18" s="51" t="s">
+      <c r="W18" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="40" t="s">
+      <c r="X18" s="57"/>
+      <c r="Y18" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="Z18" s="50" t="s">
+      <c r="Z18" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="AA18" s="51" t="s">
+      <c r="AA18" s="54" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3697,46 +3720,46 @@
       <c r="F19" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="40" t="s">
+      <c r="I19" s="33"/>
+      <c r="J19" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="L19" s="28" t="s">
+      <c r="L19" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="50" t="s">
+      <c r="Q19" s="43"/>
+      <c r="R19" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="S19" s="51" t="s">
+      <c r="S19" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="U19" s="40" t="s">
+      <c r="U19" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="V19" s="50" t="s">
+      <c r="V19" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="W19" s="51" t="s">
+      <c r="W19" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="X19" s="54"/>
-      <c r="Y19" s="40" t="s">
+      <c r="X19" s="57"/>
+      <c r="Y19" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="Z19" s="50" t="s">
+      <c r="Z19" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="AA19" s="51" t="s">
+      <c r="AA19" s="54" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3751,46 +3774,46 @@
       <c r="F20" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="40" t="s">
+      <c r="I20" s="33"/>
+      <c r="J20" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="L20" s="28" t="s">
+      <c r="L20" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="50" t="s">
+      <c r="Q20" s="43"/>
+      <c r="R20" s="53" t="s">
         <v>176</v>
       </c>
-      <c r="S20" s="51" t="s">
+      <c r="S20" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="U20" s="40" t="s">
+      <c r="U20" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="V20" s="50" t="s">
+      <c r="V20" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="W20" s="51" t="s">
+      <c r="W20" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="X20" s="54"/>
-      <c r="Y20" s="40" t="s">
+      <c r="X20" s="57"/>
+      <c r="Y20" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="Z20" s="50" t="s">
+      <c r="Z20" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="AA20" s="51" t="s">
+      <c r="AA20" s="54" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3805,45 +3828,45 @@
       <c r="F21" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="L21" s="28" t="s">
+      <c r="L21" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="50" t="s">
+      <c r="Q21" s="43"/>
+      <c r="R21" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="S21" s="51" t="s">
+      <c r="S21" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="U21" s="40" t="s">
+      <c r="U21" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="V21" s="50" t="s">
+      <c r="V21" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="W21" s="51" t="s">
+      <c r="W21" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="X21" s="54"/>
-      <c r="Y21" s="40" t="s">
+      <c r="X21" s="57"/>
+      <c r="Y21" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="Z21" s="50" t="s">
+      <c r="Z21" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="AA21" s="51" t="s">
+      <c r="AA21" s="54" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3855,52 +3878,52 @@
       <c r="D22" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="J22" s="42" t="s">
+      <c r="J22" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="K22" s="43" t="s">
+      <c r="K22" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="L22" s="44" t="s">
+      <c r="L22" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="50" t="s">
+      <c r="Q22" s="43"/>
+      <c r="R22" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="S22" s="51" t="s">
+      <c r="S22" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="U22" s="40" t="s">
+      <c r="U22" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="V22" s="50" t="s">
+      <c r="V22" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="W22" s="51" t="s">
+      <c r="W22" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="X22" s="54"/>
-      <c r="Y22" s="40" t="s">
+      <c r="X22" s="57"/>
+      <c r="Y22" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="Z22" s="50" t="s">
+      <c r="Z22" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="AA22" s="51" t="s">
+      <c r="AA22" s="54" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="2:27">
+    <row r="23" ht="13.5" spans="2:27">
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
         <v>206</v>
@@ -3908,30 +3931,30 @@
       <c r="D23" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="50" t="s">
+      <c r="Q23" s="43"/>
+      <c r="R23" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="S23" s="51" t="s">
+      <c r="S23" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="U23" s="40" t="s">
+      <c r="U23" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="V23" s="50" t="s">
+      <c r="V23" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="W23" s="51" t="s">
+      <c r="W23" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="40" t="s">
+      <c r="X23" s="57"/>
+      <c r="Y23" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="Z23" s="50" t="s">
+      <c r="Z23" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="AA23" s="51" t="s">
+      <c r="AA23" s="54" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3943,29 +3966,29 @@
       <c r="D24" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="50" t="s">
+      <c r="Q24" s="43"/>
+      <c r="R24" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="S24" s="51" t="s">
+      <c r="S24" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="U24" s="40"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="54"/>
-      <c r="Y24" s="40"/>
-      <c r="Z24" s="50"/>
-      <c r="AA24" s="51"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="54"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="53"/>
+      <c r="AA24" s="54"/>
     </row>
     <row r="25" ht="13.5" spans="2:27">
       <c r="B25" s="7"/>
@@ -3975,30 +3998,30 @@
       <c r="D25" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="50" t="s">
+      <c r="Q25" s="43"/>
+      <c r="R25" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="S25" s="51" t="s">
+      <c r="S25" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="U25" s="42" t="s">
+      <c r="U25" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="V25" s="59" t="s">
+      <c r="V25" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="W25" s="60" t="s">
+      <c r="W25" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="42" t="s">
+      <c r="X25" s="57"/>
+      <c r="Y25" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="Z25" s="59" t="s">
+      <c r="Z25" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="AA25" s="60" t="s">
+      <c r="AA25" s="63" t="s">
         <v>228</v>
       </c>
     </row>
@@ -4010,30 +4033,30 @@
       <c r="D26" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
-      <c r="J26" s="11" t="s">
+      <c r="G26" s="15"/>
+      <c r="H26" s="16"/>
+      <c r="J26" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="50" t="s">
+      <c r="K26" s="15"/>
+      <c r="L26" s="16"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="S26" s="51" t="s">
+      <c r="S26" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54"/>
-      <c r="W26" s="54"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="54"/>
-      <c r="AA26" s="54"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="57"/>
     </row>
     <row r="27" ht="13.5" spans="2:27">
       <c r="B27" s="7"/>
@@ -4043,38 +4066,38 @@
       <c r="D27" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="16" t="s">
+      <c r="L27" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="50" t="s">
+      <c r="Q27" s="43"/>
+      <c r="R27" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="S27" s="51" t="s">
+      <c r="S27" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="U27" s="54"/>
-      <c r="V27" s="54"/>
-      <c r="W27" s="54"/>
-      <c r="X27" s="54"/>
-      <c r="Y27" s="54"/>
-      <c r="Z27" s="54"/>
-      <c r="AA27" s="54"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="57"/>
+      <c r="AA27" s="57"/>
     </row>
     <row r="28" spans="2:27">
       <c r="B28" s="7"/>
@@ -4084,30 +4107,30 @@
       <c r="D28" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="19"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="19"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="50" t="s">
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="S28" s="51" t="s">
+      <c r="S28" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="U28" s="31" t="s">
+      <c r="U28" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="V28" s="52"/>
-      <c r="W28" s="53"/>
-      <c r="X28" s="54"/>
-      <c r="Y28" s="31" t="s">
+      <c r="V28" s="55"/>
+      <c r="W28" s="56"/>
+      <c r="X28" s="57"/>
+      <c r="Y28" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="53"/>
+      <c r="Z28" s="55"/>
+      <c r="AA28" s="56"/>
     </row>
     <row r="29" ht="13.5" spans="2:27">
       <c r="B29" s="7"/>
@@ -4120,45 +4143,45 @@
       <c r="F29" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="31" t="s">
         <v>250</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="K29" s="20" t="s">
+      <c r="K29" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L29" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="50" t="s">
+      <c r="Q29" s="43"/>
+      <c r="R29" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="S29" s="51" t="s">
+      <c r="S29" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="U29" s="34" t="s">
+      <c r="U29" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="V29" s="55" t="s">
+      <c r="V29" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="W29" s="56" t="s">
+      <c r="W29" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="34" t="s">
+      <c r="X29" s="57"/>
+      <c r="Y29" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="Z29" s="55" t="s">
+      <c r="Z29" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AA29" s="56" t="s">
+      <c r="AA29" s="59" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4169,45 +4192,45 @@
       <c r="F30" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="H30" s="28" t="s">
+      <c r="H30" s="31" t="s">
         <v>259</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="K30" s="20" t="s">
+      <c r="K30" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="50" t="s">
+      <c r="Q30" s="43"/>
+      <c r="R30" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="S30" s="51" t="s">
+      <c r="S30" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="U30" s="57" t="s">
+      <c r="U30" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="V30" s="48" t="s">
+      <c r="V30" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="W30" s="49" t="s">
+      <c r="W30" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="57" t="s">
+      <c r="X30" s="57"/>
+      <c r="Y30" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="Z30" s="48" t="s">
+      <c r="Z30" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="AA30" s="49" t="s">
+      <c r="AA30" s="52" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4224,45 +4247,45 @@
       <c r="F31" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="H31" s="28" t="s">
+      <c r="H31" s="31" t="s">
         <v>272</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="K31" s="20" t="s">
+      <c r="K31" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="L31" s="28" t="s">
+      <c r="L31" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="50" t="s">
+      <c r="Q31" s="43"/>
+      <c r="R31" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="S31" s="51" t="s">
+      <c r="S31" s="54" t="s">
         <v>277</v>
       </c>
-      <c r="U31" s="40" t="s">
+      <c r="U31" s="43" t="s">
         <v>257</v>
       </c>
-      <c r="V31" s="50" t="s">
+      <c r="V31" s="53" t="s">
         <v>258</v>
       </c>
-      <c r="W31" s="51" t="s">
+      <c r="W31" s="54" t="s">
         <v>278</v>
       </c>
-      <c r="X31" s="54"/>
-      <c r="Y31" s="40" t="s">
+      <c r="X31" s="57"/>
+      <c r="Y31" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="Z31" s="50" t="s">
+      <c r="Z31" s="53" t="s">
         <v>261</v>
       </c>
-      <c r="AA31" s="51" t="s">
+      <c r="AA31" s="54" t="s">
         <v>279</v>
       </c>
     </row>
@@ -4277,45 +4300,45 @@
       <c r="F32" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="H32" s="28" t="s">
+      <c r="H32" s="31" t="s">
         <v>284</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="K32" s="20" t="s">
+      <c r="K32" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="50" t="s">
+      <c r="Q32" s="43"/>
+      <c r="R32" s="53" t="s">
         <v>288</v>
       </c>
-      <c r="S32" s="51" t="s">
+      <c r="S32" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="U32" s="58" t="s">
+      <c r="U32" s="61" t="s">
         <v>290</v>
       </c>
-      <c r="V32" s="50" t="s">
+      <c r="V32" s="53" t="s">
         <v>291</v>
       </c>
-      <c r="W32" s="51" t="s">
+      <c r="W32" s="54" t="s">
         <v>292</v>
       </c>
-      <c r="X32" s="54"/>
-      <c r="Y32" s="58" t="s">
+      <c r="X32" s="57"/>
+      <c r="Y32" s="61" t="s">
         <v>273</v>
       </c>
-      <c r="Z32" s="50" t="s">
+      <c r="Z32" s="53" t="s">
         <v>274</v>
       </c>
-      <c r="AA32" s="51" t="s">
+      <c r="AA32" s="54" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4330,45 +4353,45 @@
       <c r="F33" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="H33" s="28" t="s">
+      <c r="H33" s="31" t="s">
         <v>296</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="K33" s="20" t="s">
+      <c r="K33" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="L33" s="28" t="s">
+      <c r="L33" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="50" t="s">
+      <c r="Q33" s="43"/>
+      <c r="R33" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="S33" s="51" t="s">
+      <c r="S33" s="54" t="s">
         <v>301</v>
       </c>
-      <c r="U33" s="40" t="s">
+      <c r="U33" s="43" t="s">
         <v>302</v>
       </c>
-      <c r="V33" s="50" t="s">
+      <c r="V33" s="53" t="s">
         <v>303</v>
       </c>
-      <c r="W33" s="51" t="s">
+      <c r="W33" s="54" t="s">
         <v>304</v>
       </c>
-      <c r="X33" s="54"/>
-      <c r="Y33" s="40" t="s">
+      <c r="X33" s="57"/>
+      <c r="Y33" s="43" t="s">
         <v>285</v>
       </c>
-      <c r="Z33" s="50" t="s">
+      <c r="Z33" s="53" t="s">
         <v>286</v>
       </c>
-      <c r="AA33" s="51" t="s">
+      <c r="AA33" s="54" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4379,45 +4402,45 @@
       <c r="F34" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H34" s="28" t="s">
+      <c r="H34" s="31" t="s">
         <v>306</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="K34" s="20" t="s">
+      <c r="K34" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="L34" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="50" t="s">
+      <c r="Q34" s="43"/>
+      <c r="R34" s="53" t="s">
         <v>310</v>
       </c>
-      <c r="S34" s="51" t="s">
+      <c r="S34" s="54" t="s">
         <v>311</v>
       </c>
-      <c r="U34" s="58" t="s">
+      <c r="U34" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="V34" s="50" t="s">
+      <c r="V34" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="W34" s="51" t="s">
+      <c r="W34" s="54" t="s">
         <v>312</v>
       </c>
-      <c r="X34" s="54"/>
-      <c r="Y34" s="58" t="s">
+      <c r="X34" s="57"/>
+      <c r="Y34" s="61" t="s">
         <v>313</v>
       </c>
-      <c r="Z34" s="50" t="s">
+      <c r="Z34" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="AA34" s="51" t="s">
+      <c r="AA34" s="54" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4435,45 +4458,45 @@
       <c r="F35" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="H35" s="28" t="s">
+      <c r="H35" s="31" t="s">
         <v>321</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="K35" s="20" t="s">
+      <c r="K35" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="L35" s="28" t="s">
+      <c r="L35" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="50" t="s">
+      <c r="Q35" s="43"/>
+      <c r="R35" s="53" t="s">
         <v>323</v>
       </c>
-      <c r="S35" s="51" t="s">
+      <c r="S35" s="54" t="s">
         <v>324</v>
       </c>
-      <c r="U35" s="40" t="s">
+      <c r="U35" s="43" t="s">
         <v>282</v>
       </c>
-      <c r="V35" s="50" t="s">
+      <c r="V35" s="53" t="s">
         <v>283</v>
       </c>
-      <c r="W35" s="51" t="s">
+      <c r="W35" s="54" t="s">
         <v>325</v>
       </c>
-      <c r="X35" s="54"/>
-      <c r="Y35" s="40" t="s">
+      <c r="X35" s="57"/>
+      <c r="Y35" s="43" t="s">
         <v>326</v>
       </c>
-      <c r="Z35" s="50" t="s">
+      <c r="Z35" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="AA35" s="51" t="s">
+      <c r="AA35" s="54" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4488,45 +4511,45 @@
       <c r="F36" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="31" t="s">
         <v>333</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="K36" s="20" t="s">
+      <c r="K36" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L36" s="31" t="s">
         <v>334</v>
       </c>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="50" t="s">
+      <c r="Q36" s="43"/>
+      <c r="R36" s="53" t="s">
         <v>335</v>
       </c>
-      <c r="S36" s="51" t="s">
+      <c r="S36" s="54" t="s">
         <v>336</v>
       </c>
-      <c r="U36" s="58" t="s">
+      <c r="U36" s="61" t="s">
         <v>337</v>
       </c>
-      <c r="V36" s="50" t="s">
+      <c r="V36" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="W36" s="51" t="s">
+      <c r="W36" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="X36" s="54"/>
-      <c r="Y36" s="58" t="s">
+      <c r="X36" s="57"/>
+      <c r="Y36" s="61" t="s">
         <v>297</v>
       </c>
-      <c r="Z36" s="50" t="s">
+      <c r="Z36" s="53" t="s">
         <v>298</v>
       </c>
-      <c r="AA36" s="51" t="s">
+      <c r="AA36" s="54" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4537,45 +4560,45 @@
       <c r="F37" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="H37" s="28" t="s">
+      <c r="H37" s="31" t="s">
         <v>341</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="K37" s="20" t="s">
+      <c r="K37" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="Q37" s="40"/>
-      <c r="R37" s="50" t="s">
+      <c r="Q37" s="43"/>
+      <c r="R37" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="S37" s="51" t="s">
+      <c r="S37" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="U37" s="40" t="s">
+      <c r="U37" s="43" t="s">
         <v>347</v>
       </c>
-      <c r="V37" s="50" t="s">
+      <c r="V37" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="W37" s="51" t="s">
+      <c r="W37" s="54" t="s">
         <v>349</v>
       </c>
-      <c r="X37" s="54"/>
-      <c r="Y37" s="40" t="s">
+      <c r="X37" s="57"/>
+      <c r="Y37" s="43" t="s">
         <v>307</v>
       </c>
-      <c r="Z37" s="50" t="s">
+      <c r="Z37" s="53" t="s">
         <v>308</v>
       </c>
-      <c r="AA37" s="51" t="s">
+      <c r="AA37" s="54" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4592,45 +4615,45 @@
       <c r="F38" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="H38" s="28" t="s">
+      <c r="H38" s="31" t="s">
         <v>354</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="K38" s="20" t="s">
+      <c r="K38" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="31" t="s">
         <v>357</v>
       </c>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="50" t="s">
+      <c r="Q38" s="43"/>
+      <c r="R38" s="53" t="s">
         <v>358</v>
       </c>
-      <c r="S38" s="51" t="s">
+      <c r="S38" s="54" t="s">
         <v>359</v>
       </c>
-      <c r="U38" s="58" t="s">
+      <c r="U38" s="61" t="s">
         <v>319</v>
       </c>
-      <c r="V38" s="50" t="s">
+      <c r="V38" s="53" t="s">
         <v>320</v>
       </c>
-      <c r="W38" s="51" t="s">
+      <c r="W38" s="54" t="s">
         <v>360</v>
       </c>
-      <c r="X38" s="54"/>
-      <c r="Y38" s="58" t="s">
+      <c r="X38" s="57"/>
+      <c r="Y38" s="61" t="s">
         <v>342</v>
       </c>
-      <c r="Z38" s="50" t="s">
+      <c r="Z38" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="AA38" s="51" t="s">
+      <c r="AA38" s="54" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4643,35 +4666,35 @@
         <v>363</v>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24"/>
       <c r="J39" s="7"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="21"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="50" t="s">
+      <c r="K39" s="23"/>
+      <c r="L39" s="24"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="53" t="s">
         <v>364</v>
       </c>
-      <c r="S39" s="51" t="s">
+      <c r="S39" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="U39" s="40" t="s">
+      <c r="U39" s="43" t="s">
         <v>331</v>
       </c>
-      <c r="V39" s="50" t="s">
+      <c r="V39" s="53" t="s">
         <v>332</v>
       </c>
-      <c r="W39" s="51" t="s">
+      <c r="W39" s="54" t="s">
         <v>366</v>
       </c>
-      <c r="X39" s="54"/>
-      <c r="Y39" s="40" t="s">
+      <c r="X39" s="57"/>
+      <c r="Y39" s="43" t="s">
         <v>355</v>
       </c>
-      <c r="Z39" s="50" t="s">
+      <c r="Z39" s="53" t="s">
         <v>356</v>
       </c>
-      <c r="AA39" s="51" t="s">
+      <c r="AA39" s="54" t="s">
         <v>367</v>
       </c>
     </row>
@@ -4682,35 +4705,35 @@
       <c r="F40" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="24" t="s">
         <v>368</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="K40" s="20" t="s">
+      <c r="K40" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="L40" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="50" t="s">
+      <c r="Q40" s="43"/>
+      <c r="R40" s="53" t="s">
         <v>372</v>
       </c>
-      <c r="S40" s="51" t="s">
+      <c r="S40" s="54" t="s">
         <v>373</v>
       </c>
-      <c r="U40" s="40"/>
-      <c r="V40" s="50"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="54"/>
-      <c r="Y40" s="40"/>
-      <c r="Z40" s="50"/>
-      <c r="AA40" s="51"/>
+      <c r="U40" s="43"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="54"/>
+      <c r="X40" s="57"/>
+      <c r="Y40" s="43"/>
+      <c r="Z40" s="53"/>
+      <c r="AA40" s="54"/>
     </row>
     <row r="41" spans="2:27">
       <c r="B41" s="7" t="s">
@@ -4725,45 +4748,45 @@
       <c r="F41" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="24" t="s">
         <v>376</v>
       </c>
       <c r="J41" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="K41" s="20" t="s">
+      <c r="K41" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="L41" s="21" t="s">
+      <c r="L41" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="Q41" s="40"/>
-      <c r="R41" s="50" t="s">
+      <c r="Q41" s="43"/>
+      <c r="R41" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="S41" s="51" t="s">
+      <c r="S41" s="54" t="s">
         <v>381</v>
       </c>
-      <c r="U41" s="40" t="s">
+      <c r="U41" s="43" t="s">
         <v>382</v>
       </c>
-      <c r="V41" s="50" t="s">
+      <c r="V41" s="53" t="s">
         <v>383</v>
       </c>
-      <c r="W41" s="51" t="s">
+      <c r="W41" s="54" t="s">
         <v>384</v>
       </c>
-      <c r="X41" s="54"/>
-      <c r="Y41" s="40" t="s">
+      <c r="X41" s="57"/>
+      <c r="Y41" s="43" t="s">
         <v>385</v>
       </c>
-      <c r="Z41" s="50" t="s">
+      <c r="Z41" s="53" t="s">
         <v>386</v>
       </c>
-      <c r="AA41" s="51" t="s">
+      <c r="AA41" s="54" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4778,51 +4801,51 @@
       <c r="F42" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="24" t="s">
         <v>391</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="K42" s="20" t="s">
+      <c r="K42" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="L42" s="21" t="s">
+      <c r="L42" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="50" t="s">
+      <c r="Q42" s="43"/>
+      <c r="R42" s="53" t="s">
         <v>395</v>
       </c>
-      <c r="S42" s="51" t="s">
+      <c r="S42" s="54" t="s">
         <v>396</v>
       </c>
-      <c r="U42" s="40" t="s">
+      <c r="U42" s="43" t="s">
         <v>397</v>
       </c>
-      <c r="V42" s="50" t="s">
+      <c r="V42" s="53" t="s">
         <v>398</v>
       </c>
-      <c r="W42" s="51" t="s">
+      <c r="W42" s="54" t="s">
         <v>399</v>
       </c>
-      <c r="X42" s="54"/>
-      <c r="Y42" s="40" t="s">
+      <c r="X42" s="57"/>
+      <c r="Y42" s="43" t="s">
         <v>400</v>
       </c>
-      <c r="Z42" s="50" t="s">
+      <c r="Z42" s="53" t="s">
         <v>401</v>
       </c>
-      <c r="AA42" s="51" t="s">
+      <c r="AA42" s="54" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="43" spans="2:27">
       <c r="B43" s="7"/>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="11" t="s">
         <v>115</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -4831,51 +4854,51 @@
       <c r="F43" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="24" t="s">
         <v>404</v>
       </c>
       <c r="J43" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="K43" s="20" t="s">
+      <c r="K43" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="L43" s="21" t="s">
+      <c r="L43" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="Q43" s="40"/>
-      <c r="R43" s="50" t="s">
+      <c r="Q43" s="43"/>
+      <c r="R43" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="S43" s="51" t="s">
+      <c r="S43" s="54" t="s">
         <v>409</v>
       </c>
-      <c r="U43" s="40" t="s">
+      <c r="U43" s="43" t="s">
         <v>410</v>
       </c>
-      <c r="V43" s="50" t="s">
+      <c r="V43" s="53" t="s">
         <v>411</v>
       </c>
-      <c r="W43" s="51" t="s">
+      <c r="W43" s="54" t="s">
         <v>412</v>
       </c>
-      <c r="X43" s="54"/>
-      <c r="Y43" s="40" t="s">
+      <c r="X43" s="57"/>
+      <c r="Y43" s="43" t="s">
         <v>413</v>
       </c>
-      <c r="Z43" s="50" t="s">
+      <c r="Z43" s="53" t="s">
         <v>414</v>
       </c>
-      <c r="AA43" s="51" t="s">
+      <c r="AA43" s="54" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="44" spans="2:27">
       <c r="B44" s="7"/>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="11" t="s">
         <v>121</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -4884,496 +4907,496 @@
       <c r="F44" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="24" t="s">
         <v>417</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="K44" s="20" t="s">
+      <c r="K44" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="L44" s="21" t="s">
+      <c r="L44" s="24" t="s">
         <v>420</v>
       </c>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="50" t="s">
+      <c r="Q44" s="43"/>
+      <c r="R44" s="53" t="s">
         <v>421</v>
       </c>
-      <c r="S44" s="51" t="s">
+      <c r="S44" s="54" t="s">
         <v>422</v>
       </c>
-      <c r="U44" s="40" t="s">
+      <c r="U44" s="43" t="s">
         <v>423</v>
       </c>
-      <c r="V44" s="50" t="s">
+      <c r="V44" s="53" t="s">
         <v>424</v>
       </c>
-      <c r="W44" s="51" t="s">
+      <c r="W44" s="54" t="s">
         <v>425</v>
       </c>
-      <c r="X44" s="54"/>
-      <c r="Y44" s="40" t="s">
+      <c r="X44" s="57"/>
+      <c r="Y44" s="43" t="s">
         <v>418</v>
       </c>
-      <c r="Z44" s="50" t="s">
+      <c r="Z44" s="53" t="s">
         <v>419</v>
       </c>
-      <c r="AA44" s="51" t="s">
+      <c r="AA44" s="54" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="45" ht="13.5" spans="2:27">
       <c r="B45" s="7"/>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="11" t="s">
         <v>128</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="G45" s="23" t="s">
+      <c r="G45" s="26" t="s">
         <v>411</v>
       </c>
-      <c r="H45" s="24" t="s">
+      <c r="H45" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="J45" s="22" t="s">
+      <c r="J45" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="K45" s="23" t="s">
+      <c r="K45" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="L45" s="24" t="s">
+      <c r="L45" s="27" t="s">
         <v>431</v>
       </c>
-      <c r="Q45" s="40"/>
-      <c r="R45" s="50" t="s">
+      <c r="Q45" s="43"/>
+      <c r="R45" s="53" t="s">
         <v>432</v>
       </c>
-      <c r="S45" s="51" t="s">
+      <c r="S45" s="54" t="s">
         <v>433</v>
       </c>
-      <c r="U45" s="40" t="s">
+      <c r="U45" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="V45" s="50" t="s">
+      <c r="V45" s="53" t="s">
         <v>393</v>
       </c>
-      <c r="W45" s="51" t="s">
+      <c r="W45" s="54" t="s">
         <v>434</v>
       </c>
-      <c r="X45" s="54"/>
-      <c r="Y45" s="40" t="s">
+      <c r="X45" s="57"/>
+      <c r="Y45" s="43" t="s">
         <v>435</v>
       </c>
-      <c r="Z45" s="50" t="s">
+      <c r="Z45" s="53" t="s">
         <v>436</v>
       </c>
-      <c r="AA45" s="51" t="s">
+      <c r="AA45" s="54" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="46" spans="2:27">
       <c r="B46" s="7"/>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="11" t="s">
         <v>138</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="50" t="s">
+      <c r="Q46" s="43"/>
+      <c r="R46" s="53" t="s">
         <v>439</v>
       </c>
-      <c r="S46" s="51" t="s">
+      <c r="S46" s="54" t="s">
         <v>440</v>
       </c>
-      <c r="U46" s="40" t="s">
+      <c r="U46" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="V46" s="50" t="s">
+      <c r="V46" s="53" t="s">
         <v>370</v>
       </c>
-      <c r="W46" s="51" t="s">
+      <c r="W46" s="54" t="s">
         <v>441</v>
       </c>
-      <c r="X46" s="54"/>
-      <c r="Y46" s="40" t="s">
+      <c r="X46" s="57"/>
+      <c r="Y46" s="43" t="s">
         <v>429</v>
       </c>
-      <c r="Z46" s="50" t="s">
+      <c r="Z46" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="AA46" s="51" t="s">
+      <c r="AA46" s="54" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="47" spans="2:27">
       <c r="B47" s="7"/>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="11" t="s">
         <v>150</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="50" t="s">
+      <c r="Q47" s="43"/>
+      <c r="R47" s="53" t="s">
         <v>444</v>
       </c>
-      <c r="S47" s="51" t="s">
+      <c r="S47" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="U47" s="40" t="s">
+      <c r="U47" s="43" t="s">
         <v>389</v>
       </c>
-      <c r="V47" s="50" t="s">
+      <c r="V47" s="53" t="s">
         <v>390</v>
       </c>
-      <c r="W47" s="51" t="s">
+      <c r="W47" s="54" t="s">
         <v>446</v>
       </c>
-      <c r="X47" s="54"/>
-      <c r="Y47" s="40" t="s">
+      <c r="X47" s="57"/>
+      <c r="Y47" s="43" t="s">
         <v>447</v>
       </c>
-      <c r="Z47" s="50" t="s">
+      <c r="Z47" s="53" t="s">
         <v>448</v>
       </c>
-      <c r="AA47" s="51" t="s">
+      <c r="AA47" s="54" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="48" spans="2:27">
       <c r="B48" s="7"/>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="11" t="s">
         <v>408</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="50" t="s">
+      <c r="Q48" s="43"/>
+      <c r="R48" s="53" t="s">
         <v>451</v>
       </c>
-      <c r="S48" s="51" t="s">
+      <c r="S48" s="54" t="s">
         <v>452</v>
       </c>
-      <c r="U48" s="40"/>
-      <c r="V48" s="50"/>
-      <c r="W48" s="51"/>
-      <c r="X48" s="54"/>
-      <c r="Y48" s="40"/>
-      <c r="Z48" s="50"/>
-      <c r="AA48" s="51"/>
+      <c r="U48" s="43"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="54"/>
+      <c r="X48" s="57"/>
+      <c r="Y48" s="43"/>
+      <c r="Z48" s="53"/>
+      <c r="AA48" s="54"/>
     </row>
     <row r="49" ht="13.5" spans="2:27">
       <c r="B49" s="7"/>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="11" t="s">
         <v>395</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="Q49" s="40"/>
-      <c r="R49" s="50" t="s">
+      <c r="Q49" s="43"/>
+      <c r="R49" s="53" t="s">
         <v>454</v>
       </c>
-      <c r="S49" s="51" t="s">
+      <c r="S49" s="54" t="s">
         <v>455</v>
       </c>
-      <c r="U49" s="42" t="s">
+      <c r="U49" s="45" t="s">
         <v>456</v>
       </c>
-      <c r="V49" s="59" t="s">
+      <c r="V49" s="62" t="s">
         <v>457</v>
       </c>
-      <c r="W49" s="60" t="s">
+      <c r="W49" s="63" t="s">
         <v>458</v>
       </c>
-      <c r="X49" s="54"/>
-      <c r="Y49" s="42" t="s">
+      <c r="X49" s="57"/>
+      <c r="Y49" s="45" t="s">
         <v>459</v>
       </c>
-      <c r="Z49" s="59" t="s">
+      <c r="Z49" s="62" t="s">
         <v>460</v>
       </c>
-      <c r="AA49" s="60" t="s">
+      <c r="AA49" s="63" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="50" spans="2:19">
       <c r="B50" s="7"/>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="11" t="s">
         <v>380</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="Q50" s="40"/>
-      <c r="R50" s="50" t="s">
+      <c r="Q50" s="43"/>
+      <c r="R50" s="53" t="s">
         <v>463</v>
       </c>
-      <c r="S50" s="51" t="s">
+      <c r="S50" s="54" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="51" spans="2:19">
       <c r="B51" s="7"/>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="12" t="s">
         <v>372</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="Q51" s="40"/>
-      <c r="R51" s="50" t="s">
+      <c r="Q51" s="43"/>
+      <c r="R51" s="53" t="s">
         <v>466</v>
       </c>
-      <c r="S51" s="51" t="s">
+      <c r="S51" s="54" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="52" spans="2:19">
       <c r="B52" s="7"/>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="12" t="s">
         <v>364</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="Q52" s="40"/>
-      <c r="R52" s="50"/>
-      <c r="S52" s="51"/>
+      <c r="Q52" s="43"/>
+      <c r="R52" s="53"/>
+      <c r="S52" s="54"/>
     </row>
     <row r="53" spans="2:19">
       <c r="B53" s="7"/>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="12" t="s">
         <v>358</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="Q53" s="40" t="s">
+      <c r="Q53" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="R53" s="50" t="s">
+      <c r="R53" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="S53" s="51" t="s">
+      <c r="S53" s="54" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="54" spans="2:19">
       <c r="B54" s="7"/>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="12" t="s">
         <v>345</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="Q54" s="40"/>
-      <c r="R54" s="50" t="s">
+      <c r="Q54" s="43"/>
+      <c r="R54" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="S54" s="51" t="s">
+      <c r="S54" s="54" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:19">
       <c r="B55" s="7"/>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="12" t="s">
         <v>335</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="Q55" s="40"/>
-      <c r="R55" s="50" t="s">
+      <c r="Q55" s="43"/>
+      <c r="R55" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="S55" s="51" t="s">
+      <c r="S55" s="54" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="56" spans="2:19">
       <c r="B56" s="7"/>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="12" t="s">
         <v>323</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="Q56" s="40"/>
-      <c r="R56" s="50" t="s">
+      <c r="Q56" s="43"/>
+      <c r="R56" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="S56" s="51" t="s">
+      <c r="S56" s="54" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="57" spans="2:19">
       <c r="B57" s="7"/>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="12" t="s">
         <v>310</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="Q57" s="40"/>
-      <c r="R57" s="50" t="s">
+      <c r="Q57" s="43"/>
+      <c r="R57" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="S57" s="51" t="s">
+      <c r="S57" s="54" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="58" spans="2:19">
       <c r="B58" s="7"/>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="12" t="s">
         <v>300</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="Q58" s="40"/>
-      <c r="R58" s="50" t="s">
+      <c r="Q58" s="43"/>
+      <c r="R58" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="S58" s="51" t="s">
+      <c r="S58" s="54" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="59" spans="2:19">
       <c r="B59" s="7"/>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="13" t="s">
         <v>288</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="Q59" s="40"/>
-      <c r="R59" s="50" t="s">
+      <c r="Q59" s="43"/>
+      <c r="R59" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="S59" s="51" t="s">
+      <c r="S59" s="54" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="60" spans="2:19">
       <c r="B60" s="7"/>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="13" t="s">
         <v>276</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="Q60" s="40"/>
-      <c r="R60" s="50" t="s">
+      <c r="Q60" s="43"/>
+      <c r="R60" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="S60" s="51" t="s">
+      <c r="S60" s="54" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="61" spans="2:19">
       <c r="B61" s="7"/>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="13" t="s">
         <v>263</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="Q61" s="40"/>
-      <c r="R61" s="50" t="s">
+      <c r="Q61" s="43"/>
+      <c r="R61" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="S61" s="51" t="s">
+      <c r="S61" s="54" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="62" spans="2:19">
       <c r="B62" s="7"/>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="13" t="s">
         <v>254</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="Q62" s="40"/>
-      <c r="R62" s="50" t="s">
+      <c r="Q62" s="43"/>
+      <c r="R62" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="S62" s="51" t="s">
+      <c r="S62" s="54" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="63" spans="2:19">
       <c r="B63" s="7"/>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="13" t="s">
         <v>242</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="Q63" s="40"/>
-      <c r="R63" s="50" t="s">
+      <c r="Q63" s="43"/>
+      <c r="R63" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="S63" s="51" t="s">
+      <c r="S63" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="64" spans="2:19">
       <c r="B64" s="7"/>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="13" t="s">
         <v>238</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="Q64" s="40"/>
-      <c r="R64" s="50" t="s">
+      <c r="Q64" s="43"/>
+      <c r="R64" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="S64" s="51" t="s">
+      <c r="S64" s="54" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="65" spans="2:19">
       <c r="B65" s="7"/>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="13" t="s">
         <v>233</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="Q65" s="40"/>
-      <c r="R65" s="50" t="s">
+      <c r="Q65" s="43"/>
+      <c r="R65" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="S65" s="51" t="s">
+      <c r="S65" s="54" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="66" spans="2:19">
       <c r="B66" s="7"/>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="13" t="s">
         <v>221</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="Q66" s="40"/>
-      <c r="R66" s="50" t="s">
+      <c r="Q66" s="43"/>
+      <c r="R66" s="53" t="s">
         <v>246</v>
       </c>
-      <c r="S66" s="51" t="s">
+      <c r="S66" s="54" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5385,9 +5408,9 @@
       <c r="D67" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="Q67" s="40"/>
-      <c r="R67" s="50"/>
-      <c r="S67" s="51"/>
+      <c r="Q67" s="43"/>
+      <c r="R67" s="53"/>
+      <c r="S67" s="54"/>
     </row>
     <row r="68" spans="2:19">
       <c r="B68" s="7"/>
@@ -5397,13 +5420,13 @@
       <c r="D68" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="Q68" s="40" t="s">
+      <c r="Q68" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="R68" s="50" t="s">
+      <c r="R68" s="53" t="s">
         <v>268</v>
       </c>
-      <c r="S68" s="51" t="s">
+      <c r="S68" s="54" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5415,11 +5438,11 @@
       <c r="D69" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="Q69" s="40"/>
-      <c r="R69" s="50" t="s">
+      <c r="Q69" s="43"/>
+      <c r="R69" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="S69" s="51" t="s">
+      <c r="S69" s="54" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5431,11 +5454,11 @@
       <c r="D70" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="Q70" s="40"/>
-      <c r="R70" s="50" t="s">
+      <c r="Q70" s="43"/>
+      <c r="R70" s="53" t="s">
         <v>294</v>
       </c>
-      <c r="S70" s="51" t="s">
+      <c r="S70" s="54" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5447,37 +5470,37 @@
       <c r="D71" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="Q71" s="40"/>
-      <c r="R71" s="50"/>
-      <c r="S71" s="51"/>
+      <c r="Q71" s="43"/>
+      <c r="R71" s="53"/>
+      <c r="S71" s="54"/>
     </row>
     <row r="72" ht="13.5" spans="2:19">
-      <c r="B72" s="22"/>
-      <c r="C72" s="61" t="s">
+      <c r="B72" s="25"/>
+      <c r="C72" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="D72" s="62" t="s">
+      <c r="D72" s="65" t="s">
         <v>488</v>
       </c>
-      <c r="Q72" s="40"/>
-      <c r="R72" s="50"/>
-      <c r="S72" s="51"/>
+      <c r="Q72" s="43"/>
+      <c r="R72" s="53"/>
+      <c r="S72" s="54"/>
     </row>
     <row r="73" spans="17:19">
-      <c r="Q73" s="40"/>
-      <c r="R73" s="50" t="s">
+      <c r="Q73" s="43"/>
+      <c r="R73" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="S73" s="51" t="s">
+      <c r="S73" s="54" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="74" ht="13.5" spans="17:19">
-      <c r="Q74" s="42"/>
-      <c r="R74" s="59" t="s">
+      <c r="Q74" s="45"/>
+      <c r="R74" s="62" t="s">
         <v>329</v>
       </c>
-      <c r="S74" s="60" t="s">
+      <c r="S74" s="63" t="s">
         <v>330</v>
       </c>
     </row>

</xml_diff>